<commit_message>
Update packaging and POS display scores
</commit_message>
<xml_diff>
--- a/project_ciggie/cig_regulations.xlsx
+++ b/project_ciggie/cig_regulations.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cig_regulations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -539,10 +539,10 @@
   <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:AB17"/>
+      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,8 +688,8 @@
         <v>4</v>
       </c>
       <c r="M2" s="8">
-        <f>(COUNTIF(J2:L2,"yes")*1)/3</f>
-        <v>0.33333333333333331</v>
+        <f>IF(J2="yes",1,(COUNTIF(J2:L2,"yes")*1)/3)</f>
+        <v>1</v>
       </c>
       <c r="N2" s="8">
         <v>0.5</v>
@@ -698,8 +698,8 @@
         <v>3</v>
       </c>
       <c r="Q2" s="8">
-        <f>((COUNTIF(N2:P2,"yes")*1)+(N2*1))/3</f>
-        <v>0.16666666666666666</v>
+        <f>((COUNTIF(N2:P2,"yes")*1)+(N2*1))/2</f>
+        <v>0.25</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>15</v>
@@ -761,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="8">
-        <f t="shared" ref="M3:M17" si="1">(COUNTIF(J3:L3,"yes")*1)/3</f>
+        <f t="shared" ref="M3:M17" si="1">IF(J3="yes",1,(COUNTIF(J3:L3,"yes")*1)/3)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="N3" s="9">
@@ -771,8 +771,8 @@
         <v>3</v>
       </c>
       <c r="Q3" s="8">
-        <f t="shared" ref="Q3:Q17" si="2">((COUNTIF(N3:P3,"yes")*1)+(N3*1))/3</f>
-        <v>0.16666666666666666</v>
+        <f t="shared" ref="Q3:Q17" si="2">((COUNTIF(N3:P3,"yes")*1)+(N3*1))/2</f>
+        <v>0.25</v>
       </c>
       <c r="R3" t="s">
         <v>15</v>
@@ -842,7 +842,7 @@
       </c>
       <c r="Q4" s="8">
         <f t="shared" si="2"/>
-        <v>0.11666666666666665</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="S4" t="s">
         <v>3</v>
@@ -918,7 +918,7 @@
       </c>
       <c r="Q5" s="8">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="R5" t="s">
         <v>4</v>
@@ -991,7 +991,7 @@
       </c>
       <c r="Q6" s="8">
         <f t="shared" si="2"/>
-        <v>0.13333333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="R6" t="s">
         <v>15</v>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="Q7" s="8">
         <f t="shared" si="2"/>
-        <v>9.9999999999999992E-2</v>
+        <v>0.15</v>
       </c>
       <c r="R7" t="s">
         <v>3</v>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="Q8" s="8">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="R8" t="s">
         <v>4</v>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="Q9" s="8">
         <f t="shared" si="2"/>
-        <v>0.18333333333333335</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="R9" t="s">
         <v>15</v>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="Q10" s="8">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="R10" t="s">
         <v>15</v>
@@ -1368,7 +1368,7 @@
       </c>
       <c r="Q11" s="8">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="R11" t="s">
         <v>15</v>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="Q12" s="8">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="R12" t="s">
         <v>15</v>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="Q13" s="8">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="R13" t="s">
         <v>4</v>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="Q14" s="8">
         <f t="shared" si="2"/>
-        <v>0.26666666666666666</v>
+        <v>0.4</v>
       </c>
       <c r="R14" t="s">
         <v>15</v>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="Q15" s="8">
         <f t="shared" si="2"/>
-        <v>0.11666666666666665</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="R15" t="s">
         <v>15</v>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="Q16" s="8">
         <f t="shared" si="2"/>
-        <v>0.6166666666666667</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="R16" t="s">
         <v>15</v>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="Q17" s="8">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="R17" t="s">
         <v>15</v>

</xml_diff>